<commit_message>
solicitud grafica 11-4 y escaleta actualizada
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion04/Escaleta_CN_11_04_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion04/Escaleta_CN_11_04_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos E\Aula Planeta\Autor\Física\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos E\Aula Planeta\Autor\Física\CN_11_04_CO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="228">
   <si>
     <t>Asignatura</t>
   </si>
@@ -425,21 +425,6 @@
     <t>Banco de actividades: Fenómenos ondulatorios</t>
   </si>
   <si>
-    <t>La refracción del sonido</t>
-  </si>
-  <si>
-    <t>La refracción de la luz</t>
-  </si>
-  <si>
-    <t>La difracción de la luz</t>
-  </si>
-  <si>
-    <t>La reflexión de la luz</t>
-  </si>
-  <si>
-    <t>La polarización de la luz</t>
-  </si>
-  <si>
     <t>La reflexión de las ondas luminosas y sonoras</t>
   </si>
   <si>
@@ -464,15 +449,9 @@
     <t>Refuerza tu aprendizaje: La difracción</t>
   </si>
   <si>
-    <t>Competencias: hacer un arcoiris</t>
-  </si>
-  <si>
     <t>Aprende en qué consiste la refracción</t>
   </si>
   <si>
-    <t>La reflexión del sonido</t>
-  </si>
-  <si>
     <t>Refracción de luz y sonido</t>
   </si>
   <si>
@@ -491,12 +470,6 @@
     <t>La naturaleza ondulatoria de la luz</t>
   </si>
   <si>
-    <t>Patrones de interferencia</t>
-  </si>
-  <si>
-    <t>La interferencia de ondas luminosas</t>
-  </si>
-  <si>
     <t>Mapa conceptual del tema: Fenómenos ondulatorios</t>
   </si>
   <si>
@@ -581,9 +554,6 @@
     <t>Mostrar imágenes de difracción de ondas. Mencionar la relación entre tamaño de la abertura y longitud de onda, y mencionar el principio de Huygens.</t>
   </si>
   <si>
-    <t>En las imágenes mostrar diversos ejemplos de interferencia, y hacer preguntas al respecto. Contemplar cosas como relación entre el tamaño d ela abertura y la longitud de onda.</t>
-  </si>
-  <si>
     <t>Explicar qué es, y diferenciar interferencia destructiva y constructiva. Hablar de interferencia con luz y sonido. En la de la luz, aclarar que el fenómeno no se observa si no hay fuentes en fase para que la luz interfiera; los rayos de luz se atraviezan sin alterarse. Mostrar franjas de interferencia. Hablar de interferencia por reflexión en películas delgadas.</t>
   </si>
   <si>
@@ -608,9 +578,6 @@
     <t>Preguntas diversas sobre reflexión. Se da un ángulo de incidencia y se pregunta por el de reflexión, preguntas sobre reflexión total, etc. Dra varios ejemplso de reflexíon en situaciones conocidas.</t>
   </si>
   <si>
-    <t>Actividad para reconocer aspectos generales de la refracción de las ondas.</t>
-  </si>
-  <si>
     <t>Actividad para reforzar la comprensión de la reflexión de las ondas e identificar sus leyes</t>
   </si>
   <si>
@@ -708,6 +675,39 @@
   </si>
   <si>
     <t>La reflexión y la refracción de la luz</t>
+  </si>
+  <si>
+    <t>Las leyes de la reflexión</t>
+  </si>
+  <si>
+    <t>La reflexión especular y la reflexión difusa</t>
+  </si>
+  <si>
+    <t>Actividad para reconocer aspectos generales de la refracción de las ondas</t>
+  </si>
+  <si>
+    <t>Competencias: hacer un arcoíris</t>
+  </si>
+  <si>
+    <t>Las leyes de la refracción</t>
+  </si>
+  <si>
+    <t>El índice de refracción de la luz</t>
+  </si>
+  <si>
+    <t>La polarización</t>
+  </si>
+  <si>
+    <t>Los patrones de interferencia</t>
+  </si>
+  <si>
+    <t>En las imágenes mostrar diversos ejemplos de interferencia, y hacer preguntas al respecto. Contemplar cosas como relación entre el tamaño de la abertura y la longitud de onda.</t>
+  </si>
+  <si>
+    <t>Diferentes patrones de interferencia</t>
+  </si>
+  <si>
+    <t>La relación entre la refracción y la reflexión de la luz</t>
   </si>
 </sst>
 </file>
@@ -931,34 +931,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -998,6 +980,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1308,7 +1308,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,94 +1336,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="22" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="J1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="49" t="s">
+      <c r="M1" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="29" t="s">
+      <c r="N1" s="43"/>
+      <c r="O1" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="P1" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="Q1" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="35" t="s">
+      <c r="R1" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="31" t="s">
+      <c r="S1" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="T1" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="31" t="s">
+      <c r="U1" s="46" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="22" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="44"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="38"/>
       <c r="M2" s="23" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="47"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -1441,7 +1441,7 @@
       <c r="E3" s="25"/>
       <c r="F3" s="27"/>
       <c r="G3" s="28" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H3" s="9">
         <v>1</v>
@@ -1450,7 +1450,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>20</v>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="N3" s="8"/>
       <c r="O3" s="9" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>19</v>
@@ -1472,16 +1472,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="T3" s="21" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="U3" s="19" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1498,11 +1498,11 @@
         <v>128</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>148</v>
+        <v>217</v>
       </c>
       <c r="F4" s="27"/>
       <c r="G4" s="28" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="H4" s="9">
         <v>2</v>
@@ -1511,7 +1511,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>20</v>
@@ -1524,7 +1524,7 @@
         <v>28</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>19</v>
@@ -1533,16 +1533,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="20" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="S4" s="19" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="T4" s="21" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="U4" s="19" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1559,11 +1559,11 @@
         <v>128</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>136</v>
+        <v>218</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="16" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H5" s="9">
         <v>3</v>
@@ -1572,7 +1572,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>20</v>
@@ -1585,7 +1585,7 @@
         <v>32</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>19</v>
@@ -1594,16 +1594,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="U5" s="10" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1624,7 +1624,7 @@
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="16" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="H6" s="9">
         <v>4</v>
@@ -1633,7 +1633,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>20</v>
@@ -1646,7 +1646,7 @@
         <v>52</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>19</v>
@@ -1655,16 +1655,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="U6" s="10" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1683,7 +1683,7 @@
       <c r="E7" s="13"/>
       <c r="F7" s="9"/>
       <c r="G7" s="16" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H7" s="9">
         <v>5</v>
@@ -1692,7 +1692,7 @@
         <v>19</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>20</v>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="9" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="P7" s="9" t="s">
         <v>19</v>
@@ -1714,16 +1714,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="U7" s="10" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1740,11 +1740,11 @@
         <v>129</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>133</v>
+        <v>221</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="16" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H8" s="9">
         <v>6</v>
@@ -1753,7 +1753,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>194</v>
+        <v>219</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>20</v>
@@ -1766,7 +1766,7 @@
         <v>24</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="P8" s="9" t="s">
         <v>19</v>
@@ -1775,16 +1775,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="11" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="S8" s="10" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="U8" s="10" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1801,47 +1801,51 @@
         <v>129</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>134</v>
+        <v>222</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="16" t="s">
-        <v>225</v>
+        <v>142</v>
       </c>
       <c r="H9" s="9">
         <v>7</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>226</v>
+        <v>154</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="9"/>
+      <c r="N9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>150</v>
+      </c>
       <c r="P9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="10" t="s">
-        <v>220</v>
+      <c r="Q9" s="10">
+        <v>6</v>
       </c>
       <c r="R9" s="11" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
       <c r="S9" s="10" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="U9" s="10" t="s">
-        <v>224</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1858,51 +1862,49 @@
         <v>129</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="F10" s="9"/>
+        <v>222</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>227</v>
+      </c>
       <c r="G10" s="16" t="s">
-        <v>149</v>
+        <v>214</v>
       </c>
       <c r="H10" s="9">
         <v>8</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>163</v>
+        <v>215</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L10" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M10" s="8"/>
-      <c r="N10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="O10" s="9" t="s">
-        <v>159</v>
-      </c>
+      <c r="N10" s="8"/>
+      <c r="O10" s="9"/>
       <c r="P10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="10">
-        <v>6</v>
+      <c r="Q10" s="10" t="s">
+        <v>209</v>
       </c>
       <c r="R10" s="11" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="S10" s="10" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1919,11 +1921,11 @@
         <v>129</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>137</v>
+        <v>223</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="16" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="H11" s="9">
         <v>9</v>
@@ -1932,7 +1934,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>20</v>
@@ -1945,7 +1947,7 @@
         <v>36</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="P11" s="9" t="s">
         <v>19</v>
@@ -1954,16 +1956,16 @@
         <v>6</v>
       </c>
       <c r="R11" s="11" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="S11" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="T11" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="T11" s="12" t="s">
-        <v>215</v>
-      </c>
       <c r="U11" s="10" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1984,7 +1986,7 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="16" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H12" s="9">
         <v>10</v>
@@ -1993,7 +1995,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>20</v>
@@ -2006,7 +2008,7 @@
         <v>52</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="P12" s="9" t="s">
         <v>19</v>
@@ -2015,16 +2017,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="S12" s="10" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="T12" s="12" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2043,7 +2045,7 @@
       <c r="E13" s="25"/>
       <c r="F13" s="9"/>
       <c r="G13" s="16" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H13" s="9">
         <v>11</v>
@@ -2052,7 +2054,7 @@
         <v>19</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>20</v>
@@ -2065,7 +2067,7 @@
       </c>
       <c r="N13" s="8"/>
       <c r="O13" s="9" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="P13" s="9" t="s">
         <v>19</v>
@@ -2074,16 +2076,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="11" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="S13" s="10" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="T13" s="12" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="U13" s="10" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2099,12 +2101,10 @@
       <c r="D14" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="E14" s="25" t="s">
-        <v>135</v>
-      </c>
+      <c r="E14" s="25"/>
       <c r="F14" s="9"/>
       <c r="G14" s="16" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="H14" s="9">
         <v>12</v>
@@ -2113,7 +2113,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>20</v>
@@ -2126,7 +2126,7 @@
         <v>40</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="P14" s="9" t="s">
         <v>19</v>
@@ -2135,16 +2135,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="11" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="T14" s="12" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2160,12 +2160,10 @@
       <c r="D15" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="E15" s="13" t="s">
-        <v>135</v>
-      </c>
+      <c r="E15" s="13"/>
       <c r="F15" s="9"/>
       <c r="G15" s="16" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="H15" s="9">
         <v>13</v>
@@ -2174,7 +2172,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>20</v>
@@ -2187,7 +2185,7 @@
         <v>32</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="P15" s="9" t="s">
         <v>20</v>
@@ -2196,16 +2194,16 @@
         <v>6</v>
       </c>
       <c r="R15" s="11" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="U15" s="10" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2226,7 +2224,7 @@
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="16" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="H16" s="9">
         <v>14</v>
@@ -2235,7 +2233,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>20</v>
@@ -2248,7 +2246,7 @@
         <v>52</v>
       </c>
       <c r="O16" s="9" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="P16" s="9" t="s">
         <v>19</v>
@@ -2257,16 +2255,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="U16" s="10" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2285,7 +2283,7 @@
       <c r="E17" s="13"/>
       <c r="F17" s="9"/>
       <c r="G17" s="16" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="H17" s="9">
         <v>15</v>
@@ -2294,7 +2292,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>20</v>
@@ -2307,7 +2305,7 @@
       </c>
       <c r="N17" s="8"/>
       <c r="O17" s="9" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="P17" s="9" t="s">
         <v>19</v>
@@ -2316,16 +2314,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="S17" s="10" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="T17" s="12" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="U17" s="10" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2342,11 +2340,11 @@
         <v>130</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>156</v>
+        <v>224</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="16" t="s">
-        <v>155</v>
+        <v>226</v>
       </c>
       <c r="H18" s="9">
         <v>16</v>
@@ -2355,7 +2353,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>20</v>
@@ -2368,7 +2366,7 @@
         <v>32</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>185</v>
+        <v>225</v>
       </c>
       <c r="P18" s="9" t="s">
         <v>19</v>
@@ -2377,16 +2375,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2403,11 +2401,11 @@
         <v>130</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>156</v>
+        <v>224</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="16" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="H19" s="9">
         <v>17</v>
@@ -2416,7 +2414,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>20</v>
@@ -2429,7 +2427,7 @@
         <v>36</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="P19" s="9" t="s">
         <v>20</v>
@@ -2438,16 +2436,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="S19" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="T19" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="T19" s="12" t="s">
-        <v>215</v>
-      </c>
       <c r="U19" s="10" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2468,7 +2466,7 @@
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="16" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="H20" s="9">
         <v>18</v>
@@ -2477,7 +2475,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>20</v>
@@ -2490,7 +2488,7 @@
         <v>52</v>
       </c>
       <c r="O20" s="9" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="P20" s="9" t="s">
         <v>19</v>
@@ -2499,16 +2497,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="S20" s="10" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="U20" s="10" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2527,7 +2525,7 @@
       <c r="E21" s="13"/>
       <c r="F21" s="9"/>
       <c r="G21" s="16" t="s">
-        <v>146</v>
+        <v>220</v>
       </c>
       <c r="H21" s="9">
         <v>19</v>
@@ -2536,7 +2534,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>19</v>
@@ -2551,19 +2549,19 @@
         <v>19</v>
       </c>
       <c r="Q21" s="10" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="R21" s="11" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="S21" s="10" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="T21" s="12" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="U21" s="10" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2591,7 +2589,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>20</v>
@@ -2636,7 +2634,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>20</v>
@@ -2656,16 +2654,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="11" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="S23" s="10" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="T23" s="12" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="U23" s="10" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2693,7 +2691,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>20</v>
@@ -2713,16 +2711,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="11" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="S24" s="10" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="T24" s="12" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="U24" s="10" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4471,6 +4469,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4485,12 +4489,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>